<commit_message>
Update schedule file: Y2_B2526_Blood_&_lymphatics_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y2_B2526_Blood_&_lymphatics_schedule.xlsx
+++ b/modules_schedules/Y2_B2526_Blood_&_lymphatics_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2057,6 +2057,531 @@
         <v>75</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>biochemistry cbl</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E47" s="7" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E49" s="7" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="F49" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E51" s="7" t="inlineStr">
+        <is>
+          <t>14/10/2025</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G51" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>parasitology</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>parasitology</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>parasitology</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>12/10/2025</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B55" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C55" s="6" t="inlineStr">
+        <is>
+          <t>parasitology</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C57" s="6" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E57" s="7" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>05/10/2025</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E59" s="7" t="inlineStr">
+        <is>
+          <t>14/10/2025</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
+        <is>
+          <t>07/10/2025</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload Y2_B2526_Blood_&_lymphatics_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y2_B2526_Blood_&_lymphatics_schedule.xlsx
+++ b/modules_schedules/Y2_B2526_Blood_&_lymphatics_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03198C69-3330-4BEF-80F7-AC83128054FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5087C5D5-4461-43C8-B99A-E193BAE97AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blood_&amp;_lymphatics" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="53">
   <si>
     <t>Year</t>
   </si>
@@ -58,9 +58,6 @@
     <t>08:00:00</t>
   </si>
   <si>
-    <t>biochemistry cbl</t>
-  </si>
-  <si>
     <t>02/10/2025</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>physiology</t>
   </si>
   <si>
-    <t>pos</t>
-  </si>
-  <si>
     <t>30/09/2025</t>
   </si>
   <si>
@@ -179,6 +173,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Parasitology SGD/POS</t>
+  </si>
+  <si>
+    <t>Biochemistry Lab/CBL</t>
   </si>
 </sst>
 </file>
@@ -570,13 +570,13 @@
   <dimension ref="A1:G154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
@@ -636,16 +636,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="9">
         <v>120</v>
@@ -659,13 +659,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="4">
         <v>0.41666666666666669</v>
@@ -682,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6">
         <v>2</v>
@@ -705,16 +705,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="G6" s="5">
         <v>120</v>
@@ -728,13 +728,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>11</v>
@@ -751,16 +751,16 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G8" s="5">
         <v>120</v>
@@ -774,16 +774,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9">
         <v>120</v>
@@ -797,13 +797,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2">
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4">
         <v>0.33333333333333331</v>
@@ -820,16 +820,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="9">
         <v>120</v>
@@ -843,16 +843,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="5">
         <v>120</v>
@@ -866,13 +866,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="6">
         <v>2</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="8">
         <v>0.5</v>
@@ -889,13 +889,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -912,16 +912,16 @@
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="9">
         <v>120</v>
@@ -935,16 +935,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2">
         <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="5">
         <v>120</v>
@@ -958,16 +958,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="9">
         <v>75</v>
@@ -981,13 +981,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>11</v>
@@ -1001,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -1024,19 +1024,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="5">
         <v>120</v>
@@ -1047,16 +1047,16 @@
         <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>11</v>
@@ -1070,10 +1070,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -1093,16 +1093,16 @@
         <v>7</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="F23" s="8">
         <v>0.5</v>
@@ -1116,19 +1116,19 @@
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24" s="5">
         <v>120</v>
@@ -1139,16 +1139,16 @@
         <v>7</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>11</v>
@@ -1162,16 +1162,16 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2">
         <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1185,16 +1185,16 @@
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="6">
         <v>4</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" s="8">
         <v>0.33333333333333331</v>
@@ -1208,16 +1208,16 @@
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="4">
         <v>0.41666666666666669</v>
@@ -1231,19 +1231,19 @@
         <v>7</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="F29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G29" s="9">
         <v>120</v>
@@ -1254,19 +1254,19 @@
         <v>7</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G30" s="5">
         <v>120</v>
@@ -1277,16 +1277,16 @@
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="6">
         <v>3</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31" s="8">
         <v>0.41666666666666669</v>
@@ -1300,19 +1300,19 @@
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" s="5">
         <v>120</v>
@@ -1323,19 +1323,19 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="G33" s="9">
         <v>120</v>
@@ -1346,19 +1346,19 @@
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" s="5">
         <v>75</v>
@@ -1369,16 +1369,16 @@
         <v>7</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D35" s="6">
         <v>2</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" s="8">
         <v>0.5</v>
@@ -1392,7 +1392,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" s="4">
         <v>0.41666666666666669</v>
@@ -1415,16 +1415,16 @@
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D37" s="6">
         <v>1</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>11</v>
@@ -1438,19 +1438,19 @@
         <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G38" s="5">
         <v>120</v>
@@ -1461,16 +1461,16 @@
         <v>7</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D39" s="6">
         <v>2</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F39" s="8">
         <v>0.41666666666666669</v>
@@ -1484,16 +1484,16 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F40" s="4">
         <v>0.5</v>
@@ -1507,19 +1507,19 @@
         <v>7</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="E41" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" s="9">
         <v>120</v>
@@ -1530,16 +1530,16 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F42" s="4">
         <v>0.5</v>
@@ -1553,19 +1553,19 @@
         <v>7</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="6">
         <v>3</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G43" s="9">
         <v>120</v>
@@ -1576,16 +1576,16 @@
         <v>7</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="2">
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F44" s="4">
         <v>0.5</v>
@@ -1599,16 +1599,16 @@
         <v>7</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D45" s="6">
         <v>1</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F45" s="8">
         <v>0.41666666666666669</v>
@@ -1622,19 +1622,19 @@
         <v>7</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G46" s="5">
         <v>120</v>
@@ -1645,10 +1645,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="6">
         <v>2</v>
@@ -1668,19 +1668,19 @@
         <v>7</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" s="2">
         <v>3</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="G48" s="5">
         <v>120</v>
@@ -1691,19 +1691,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C49" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="F49" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G49" s="9">
         <v>120</v>
@@ -1714,19 +1714,19 @@
         <v>7</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D50" s="2">
         <v>2</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G50" s="5">
         <v>120</v>
@@ -1737,16 +1737,16 @@
         <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D51" s="6">
         <v>1</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>11</v>
@@ -1760,16 +1760,16 @@
         <v>7</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D52" s="2">
         <v>2</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F52" s="4">
         <v>0.45833333333333331</v>
@@ -1783,7 +1783,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>9</v>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F53" s="8">
         <v>0.45833333333333331</v>
@@ -1806,19 +1806,19 @@
         <v>7</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G54" s="5">
         <v>120</v>
@@ -1829,16 +1829,16 @@
         <v>7</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>11</v>
@@ -1852,19 +1852,19 @@
         <v>7</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G56" s="5">
         <v>120</v>
@@ -1875,19 +1875,19 @@
         <v>7</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G57" s="9">
         <v>120</v>
@@ -1898,19 +1898,19 @@
         <v>7</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E58" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G58" s="5">
         <v>120</v>
@@ -1921,19 +1921,19 @@
         <v>7</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="G59" s="9">
         <v>120</v>
@@ -1944,16 +1944,16 @@
         <v>7</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D60" s="2">
         <v>3</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F60" s="4">
         <v>0.41666666666666669</v>
@@ -1967,16 +1967,16 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" s="6">
         <v>4</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F61" s="8">
         <v>0.5</v>
@@ -1990,16 +1990,16 @@
         <v>7</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F62" s="4">
         <v>0.41666666666666669</v>
@@ -2013,10 +2013,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D63" s="6">
         <v>1</v>
@@ -2036,16 +2036,16 @@
         <v>7</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D64" s="2">
         <v>2</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F64" s="4">
         <v>0.5</v>
@@ -2059,19 +2059,19 @@
         <v>7</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D65" s="6">
         <v>3</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G65" s="9">
         <v>120</v>
@@ -2082,19 +2082,19 @@
         <v>7</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F66" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G66" s="5">
         <v>120</v>
@@ -2105,16 +2105,16 @@
         <v>7</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D67" s="6">
         <v>2</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>11</v>
@@ -2128,19 +2128,19 @@
         <v>7</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="G68" s="5">
         <v>75</v>
@@ -2151,10 +2151,10 @@
         <v>7</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D69" s="6">
         <v>2</v>
@@ -2174,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>9</v>
@@ -2197,10 +2197,10 @@
         <v>7</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D71" s="6">
         <v>1</v>
@@ -2220,19 +2220,19 @@
         <v>7</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G72" s="5">
         <v>120</v>
@@ -2243,16 +2243,16 @@
         <v>7</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D73" s="6">
         <v>2</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F73" s="8">
         <v>0.5</v>
@@ -2266,19 +2266,19 @@
         <v>7</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74" s="2">
         <v>3</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G74" s="5">
         <v>120</v>
@@ -2289,19 +2289,19 @@
         <v>7</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D75" s="6">
         <v>1</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G75" s="9">
         <v>120</v>
@@ -2312,10 +2312,10 @@
         <v>7</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
@@ -2324,7 +2324,7 @@
         <v>45937</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G76" s="5">
         <v>120</v>
@@ -2335,19 +2335,19 @@
         <v>7</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G77" s="9">
         <v>120</v>
@@ -2358,10 +2358,10 @@
         <v>7</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" s="2">
         <v>3</v>
@@ -2381,16 +2381,16 @@
         <v>7</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D79" s="6">
         <v>4</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F79" s="8">
         <v>0.41666666666666669</v>
@@ -2404,16 +2404,16 @@
         <v>7</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F80" s="4">
         <v>0.5</v>
@@ -2427,19 +2427,19 @@
         <v>7</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D81" s="6">
         <v>1</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G81" s="9">
         <v>120</v>
@@ -2450,16 +2450,16 @@
         <v>7</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D82" s="2">
         <v>2</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F82" s="4">
         <v>0.5</v>
@@ -2473,16 +2473,16 @@
         <v>7</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D83" s="6">
         <v>1</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>11</v>
@@ -2496,16 +2496,16 @@
         <v>7</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D84" s="2">
         <v>2</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F84" s="4">
         <v>0.5</v>
@@ -2519,16 +2519,16 @@
         <v>7</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D85" s="6">
         <v>1</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F85" s="8">
         <v>0.625</v>
@@ -2542,19 +2542,19 @@
         <v>7</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D86" s="2">
         <v>2</v>
       </c>
       <c r="E86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G86" s="5">
         <v>75</v>
@@ -2565,7 +2565,7 @@
         <v>7</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>9</v>
@@ -2588,16 +2588,16 @@
         <v>7</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F88" s="4">
         <v>0.5</v>
@@ -2611,19 +2611,19 @@
         <v>7</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D89" s="6">
         <v>2</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G89" s="9">
         <v>120</v>
@@ -2634,16 +2634,16 @@
         <v>7</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D90" s="2">
         <v>3</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F90" s="4">
         <v>0.5</v>
@@ -2657,16 +2657,16 @@
         <v>7</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D91" s="6">
         <v>1</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F91" s="8">
         <v>0.5</v>
@@ -2680,16 +2680,16 @@
         <v>7</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D92" s="2">
         <v>1</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F92" s="4">
         <v>0.5</v>
@@ -2703,16 +2703,16 @@
         <v>7</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D93" s="6">
         <v>2</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>11</v>
@@ -2726,16 +2726,16 @@
         <v>7</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D94" s="2">
         <v>3</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F94" s="4">
         <v>0.41666666666666669</v>
@@ -2749,16 +2749,16 @@
         <v>7</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D95" s="6">
         <v>1</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>11</v>
@@ -2772,19 +2772,19 @@
         <v>7</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G96" s="5">
         <v>120</v>
@@ -2795,19 +2795,19 @@
         <v>7</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D97" s="6">
         <v>1</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G97" s="9">
         <v>120</v>
@@ -2818,19 +2818,19 @@
         <v>7</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D98" s="2">
         <v>2</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G98" s="5">
         <v>120</v>
@@ -2841,16 +2841,16 @@
         <v>7</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D99" s="6">
         <v>2</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F99" s="8">
         <v>0.5</v>
@@ -2864,19 +2864,19 @@
         <v>7</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D100" s="2">
         <v>1</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G100" s="5">
         <v>120</v>
@@ -2887,16 +2887,16 @@
         <v>7</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D101" s="6">
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F101" s="8">
         <v>0.41666666666666669</v>
@@ -2910,19 +2910,19 @@
         <v>7</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G102" s="5">
         <v>75</v>
@@ -2933,16 +2933,16 @@
         <v>7</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D103" s="6">
         <v>2</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F103" s="8">
         <v>0.58333333333333337</v>
@@ -2956,7 +2956,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>
@@ -2965,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F104" s="4" t="s">
         <v>11</v>
@@ -2979,19 +2979,19 @@
         <v>7</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D105" s="6">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E105" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="F105" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G105" s="9">
         <v>120</v>
@@ -3002,10 +3002,10 @@
         <v>7</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D106" s="2">
         <v>1</v>
@@ -3025,19 +3025,19 @@
         <v>7</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D107" s="6">
         <v>2</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G107" s="9">
         <v>120</v>
@@ -3048,16 +3048,16 @@
         <v>7</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D108" s="2">
         <v>1</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F108" s="4">
         <v>0.41666666666666669</v>
@@ -3071,16 +3071,16 @@
         <v>7</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D109" s="6">
         <v>1</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>11</v>
@@ -3094,10 +3094,10 @@
         <v>7</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D110" s="2">
         <v>2</v>
@@ -3117,16 +3117,16 @@
         <v>7</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D111" s="6">
         <v>3</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F111" s="8">
         <v>0.41666666666666669</v>
@@ -3140,19 +3140,19 @@
         <v>7</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D112" s="2">
         <v>4</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G112" s="5">
         <v>120</v>
@@ -3163,16 +3163,16 @@
         <v>7</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D113" s="6">
         <v>1</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F113" s="8">
         <v>0.5</v>
@@ -3186,16 +3186,16 @@
         <v>7</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F114" s="4" t="s">
         <v>11</v>
@@ -3209,16 +3209,16 @@
         <v>7</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D115" s="6">
         <v>2</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F115" s="8" t="s">
         <v>11</v>
@@ -3232,16 +3232,16 @@
         <v>7</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D116" s="2">
         <v>3</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F116" s="4">
         <v>0.33333333333333331</v>
@@ -3255,19 +3255,19 @@
         <v>7</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D117" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E117" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E117" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="F117" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G117" s="9">
         <v>120</v>
@@ -3278,16 +3278,16 @@
         <v>7</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D118" s="2">
         <v>2</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F118" s="4">
         <v>0.5</v>
@@ -3301,19 +3301,19 @@
         <v>7</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G119" s="9">
         <v>75</v>
@@ -3324,16 +3324,16 @@
         <v>7</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D120" s="2">
         <v>2</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F120" s="4">
         <v>0.41666666666666669</v>
@@ -3347,7 +3347,7 @@
         <v>7</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>9</v>
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F121" s="8">
         <v>0.375</v>
@@ -3370,16 +3370,16 @@
         <v>7</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D122" s="2">
         <v>1</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F122" s="4" t="s">
         <v>11</v>
@@ -3393,10 +3393,10 @@
         <v>7</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D123" s="6">
         <v>1</v>
@@ -3416,16 +3416,16 @@
         <v>7</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D124" s="2">
         <v>2</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F124" s="4">
         <v>0.5</v>
@@ -3439,16 +3439,16 @@
         <v>7</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D125" s="6">
         <v>1</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F125" s="8">
         <v>0.33333333333333331</v>
@@ -3462,19 +3462,19 @@
         <v>7</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D126" s="2">
         <v>1</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G126" s="5">
         <v>120</v>
@@ -3485,10 +3485,10 @@
         <v>7</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D127" s="6">
         <v>2</v>
@@ -3508,16 +3508,16 @@
         <v>7</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D128" s="2">
         <v>3</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F128" s="4">
         <v>0.41666666666666669</v>
@@ -3531,19 +3531,19 @@
         <v>7</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D129" s="6">
         <v>4</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G129" s="9">
         <v>120</v>
@@ -3554,19 +3554,19 @@
         <v>7</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D130" s="2">
         <v>1</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G130" s="5">
         <v>120</v>
@@ -3577,19 +3577,19 @@
         <v>7</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D131" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E131" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E131" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="F131" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G131" s="9">
         <v>120</v>
@@ -3600,16 +3600,16 @@
         <v>7</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D132" s="2">
         <v>2</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F132" s="4">
         <v>0.41666666666666669</v>
@@ -3623,16 +3623,16 @@
         <v>7</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D133" s="6">
         <v>3</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F133" s="8">
         <v>0.41666666666666669</v>
@@ -3646,16 +3646,16 @@
         <v>7</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D134" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E134" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="F134" s="4" t="s">
         <v>11</v>
@@ -3669,19 +3669,19 @@
         <v>7</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D135" s="6">
         <v>2</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G135" s="9">
         <v>120</v>
@@ -3692,16 +3692,16 @@
         <v>7</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D136" s="2">
         <v>2</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F136" s="4">
         <v>0.375</v>
@@ -3715,19 +3715,19 @@
         <v>7</v>
       </c>
       <c r="B137" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D137" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C137" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D137" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="E137" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G137" s="9">
         <v>75</v>
@@ -3738,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>9</v>
@@ -3747,10 +3747,10 @@
         <v>1</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G138" s="5">
         <v>75</v>
@@ -3761,19 +3761,19 @@
         <v>7</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G139" s="9">
         <v>120</v>
@@ -3784,19 +3784,19 @@
         <v>7</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G140" s="5">
         <v>120</v>
@@ -3807,19 +3807,19 @@
         <v>7</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G141" s="9">
         <v>120</v>
@@ -3830,19 +3830,19 @@
         <v>7</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D142" s="2">
         <v>1</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G142" s="5">
         <v>120</v>
@@ -3853,16 +3853,16 @@
         <v>7</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C143" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D143" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D143" s="6" t="s">
+      <c r="E143" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E143" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F143" s="8" t="s">
         <v>11</v>
@@ -3876,19 +3876,19 @@
         <v>7</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G144" s="5">
         <v>120</v>
@@ -3899,19 +3899,19 @@
         <v>7</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D145" s="6">
         <v>3</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G145" s="9">
         <v>120</v>
@@ -3922,19 +3922,19 @@
         <v>7</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D146" s="2">
         <v>4</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G146" s="5">
         <v>120</v>
@@ -3945,16 +3945,16 @@
         <v>7</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D147" s="6">
         <v>1</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F147" s="8" t="s">
         <v>11</v>
@@ -3968,16 +3968,16 @@
         <v>7</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F148" s="4" t="s">
         <v>11</v>
@@ -3991,16 +3991,16 @@
         <v>7</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F149" s="8" t="s">
         <v>11</v>
@@ -4014,19 +4014,19 @@
         <v>7</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G150" s="5">
         <v>120</v>
@@ -4037,16 +4037,16 @@
         <v>7</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D151" s="6">
         <v>4</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F151" s="8">
         <v>0.41666666666666669</v>
@@ -4060,16 +4060,16 @@
         <v>7</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D152" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>11</v>
@@ -4083,16 +4083,16 @@
         <v>7</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D153" s="6">
         <v>1</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F153" s="8" t="s">
         <v>11</v>
@@ -4106,10 +4106,10 @@
         <v>7</v>
       </c>
       <c r="B154" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D154" s="2">
         <v>1</v>

</xml_diff>